<commit_message>
versão 2 dos minicursos do ERIN
</commit_message>
<xml_diff>
--- a/ERIN minicursos.xlsx
+++ b/ERIN minicursos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Minicursos</t>
   </si>
@@ -23,6 +23,9 @@
   </si>
   <si>
     <t>horas</t>
+  </si>
+  <si>
+    <t>mc8</t>
   </si>
 </sst>
 </file>
@@ -392,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,6 +422,14 @@
         <v>8</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>